<commit_message>
mod transformations testing excel
</commit_message>
<xml_diff>
--- a/croatia/data/ssp_croatia_transformation_2024_12_13_testing_ver.xlsx
+++ b/croatia/data/ssp_croatia_transformation_2024_12_13_testing_ver.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarob\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D259260-63D5-465A-AC21-A14212E48D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D74EE1E-0633-4894-B59E-4ECD7385C4F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2234,7 +2234,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2367,6 +2367,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2741,9 +2744,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1048523"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M17" sqref="M17:M18"/>
+      <selection pane="topRight" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -2908,9 +2911,7 @@
       </c>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
-      <c r="O3" s="16">
-        <v>0.5</v>
-      </c>
+      <c r="O3" s="16"/>
       <c r="P3" s="15"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="28" t="s">
@@ -2979,22 +2980,22 @@
       </c>
     </row>
     <row r="5" spans="1:20" ht="143.44999999999999" customHeight="1">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="66" t="s">
+      <c r="C5" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="66" t="s">
+      <c r="D5" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="68" t="s">
+      <c r="E5" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="66" t="s">
+      <c r="F5" s="67" t="s">
         <v>26</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -3010,37 +3011,37 @@
       <c r="J5" s="2">
         <v>2030</v>
       </c>
-      <c r="K5" s="58">
-        <v>0</v>
-      </c>
-      <c r="L5" s="58">
+      <c r="K5" s="59">
+        <v>0</v>
+      </c>
+      <c r="L5" s="59">
         <v>1</v>
       </c>
-      <c r="M5" s="58">
+      <c r="M5" s="59">
         <v>0.4</v>
       </c>
-      <c r="N5" s="58">
+      <c r="N5" s="59">
         <v>0.4</v>
       </c>
-      <c r="O5" s="59">
+      <c r="O5" s="60">
         <v>0.95</v>
       </c>
-      <c r="P5" s="61" t="s">
+      <c r="P5" s="62" t="s">
         <v>403</v>
       </c>
-      <c r="Q5" s="61" t="s">
+      <c r="Q5" s="62" t="s">
         <v>403</v>
       </c>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
     </row>
     <row r="6" spans="1:20" ht="72" customHeight="1">
-      <c r="A6" s="67"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="67"/>
+      <c r="A6" s="68"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="68"/>
       <c r="G6" s="7" t="s">
         <v>388</v>
       </c>
@@ -3054,13 +3055,13 @@
       <c r="J6" s="2">
         <v>2030</v>
       </c>
-      <c r="K6" s="58"/>
-      <c r="L6" s="58"/>
-      <c r="M6" s="58"/>
-      <c r="N6" s="58"/>
-      <c r="O6" s="59"/>
-      <c r="P6" s="61"/>
-      <c r="Q6" s="61"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="59"/>
+      <c r="N6" s="59"/>
+      <c r="O6" s="60"/>
+      <c r="P6" s="62"/>
+      <c r="Q6" s="62"/>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
     </row>
@@ -3162,22 +3163,22 @@
       </c>
     </row>
     <row r="9" spans="1:20" ht="72" customHeight="1">
-      <c r="A9" s="66" t="s">
+      <c r="A9" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="66" t="s">
+      <c r="B9" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="66" t="s">
+      <c r="C9" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="66" t="s">
+      <c r="D9" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="68" t="s">
+      <c r="E9" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="66" t="s">
+      <c r="F9" s="67" t="s">
         <v>42</v>
       </c>
       <c r="G9" s="7" t="s">
@@ -3193,28 +3194,28 @@
       <c r="J9" s="2">
         <v>2030</v>
       </c>
-      <c r="K9" s="58">
-        <v>0</v>
-      </c>
-      <c r="L9" s="58">
+      <c r="K9" s="59">
+        <v>0</v>
+      </c>
+      <c r="L9" s="59">
         <v>1</v>
       </c>
-      <c r="M9" s="58">
+      <c r="M9" s="59">
         <v>0.3</v>
       </c>
-      <c r="N9" s="58">
+      <c r="N9" s="59">
         <v>0.3</v>
       </c>
-      <c r="O9" s="59">
+      <c r="O9" s="60">
         <v>0.6</v>
       </c>
-      <c r="P9" s="61" t="s">
+      <c r="P9" s="62" t="s">
         <v>427</v>
       </c>
-      <c r="Q9" s="61" t="s">
+      <c r="Q9" s="62" t="s">
         <v>427</v>
       </c>
-      <c r="R9" s="56" t="s">
+      <c r="R9" s="57" t="s">
         <v>353</v>
       </c>
       <c r="S9" s="2" t="s">
@@ -3222,12 +3223,12 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="72" customHeight="1">
-      <c r="A10" s="67"/>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="67"/>
+      <c r="A10" s="68"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="68"/>
       <c r="G10" s="2" t="s">
         <v>43</v>
       </c>
@@ -3241,14 +3242,14 @@
       <c r="J10" s="2">
         <v>2030</v>
       </c>
-      <c r="K10" s="58"/>
-      <c r="L10" s="58"/>
-      <c r="M10" s="58"/>
-      <c r="N10" s="58"/>
-      <c r="O10" s="59"/>
-      <c r="P10" s="61"/>
-      <c r="Q10" s="61"/>
-      <c r="R10" s="57"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="59"/>
+      <c r="M10" s="59"/>
+      <c r="N10" s="59"/>
+      <c r="O10" s="60"/>
+      <c r="P10" s="62"/>
+      <c r="Q10" s="62"/>
+      <c r="R10" s="58"/>
       <c r="S10" s="2" t="s">
         <v>645</v>
       </c>
@@ -3458,22 +3459,22 @@
       </c>
     </row>
     <row r="15" spans="1:20" ht="72" customHeight="1">
-      <c r="A15" s="72" t="s">
+      <c r="A15" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="72" t="s">
+      <c r="B15" s="73" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="72" t="s">
+      <c r="C15" s="73" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="72" t="s">
+      <c r="D15" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="E15" s="73" t="s">
+      <c r="E15" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="F15" s="72" t="s">
+      <c r="F15" s="73" t="s">
         <v>65</v>
       </c>
       <c r="G15" s="7" t="s">
@@ -3489,23 +3490,25 @@
       <c r="J15" s="2">
         <v>2026</v>
       </c>
-      <c r="K15" s="58">
-        <v>0</v>
-      </c>
-      <c r="L15" s="58" t="s">
+      <c r="K15" s="59">
+        <v>0</v>
+      </c>
+      <c r="L15" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="M15" s="58"/>
-      <c r="N15" s="59">
+      <c r="M15" s="59">
+        <v>0.25</v>
+      </c>
+      <c r="N15" s="60">
         <v>0.45</v>
       </c>
-      <c r="O15" s="59">
+      <c r="O15" s="60">
         <v>0.6</v>
       </c>
-      <c r="P15" s="61" t="s">
+      <c r="P15" s="62" t="s">
         <v>428</v>
       </c>
-      <c r="Q15" s="64" t="s">
+      <c r="Q15" s="65" t="s">
         <v>405</v>
       </c>
       <c r="R15" s="28" t="s">
@@ -3516,12 +3519,12 @@
       </c>
     </row>
     <row r="16" spans="1:20" ht="72" customHeight="1">
-      <c r="A16" s="72"/>
-      <c r="B16" s="72"/>
-      <c r="C16" s="72"/>
-      <c r="D16" s="72"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="72"/>
+      <c r="A16" s="73"/>
+      <c r="B16" s="73"/>
+      <c r="C16" s="73"/>
+      <c r="D16" s="73"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="73"/>
       <c r="G16" s="7" t="s">
         <v>386</v>
       </c>
@@ -3535,33 +3538,33 @@
       <c r="J16" s="2">
         <v>2030</v>
       </c>
-      <c r="K16" s="58"/>
-      <c r="L16" s="58"/>
-      <c r="M16" s="58"/>
-      <c r="N16" s="59"/>
-      <c r="O16" s="59"/>
-      <c r="P16" s="61"/>
-      <c r="Q16" s="65"/>
+      <c r="K16" s="59"/>
+      <c r="L16" s="59"/>
+      <c r="M16" s="59"/>
+      <c r="N16" s="60"/>
+      <c r="O16" s="60"/>
+      <c r="P16" s="62"/>
+      <c r="Q16" s="66"/>
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
     </row>
     <row r="17" spans="1:20" ht="72" customHeight="1">
-      <c r="A17" s="56" t="s">
+      <c r="A17" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="56" t="s">
+      <c r="B17" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="56" t="s">
+      <c r="C17" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="D17" s="56" t="s">
+      <c r="D17" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="70" t="s">
+      <c r="E17" s="71" t="s">
         <v>68</v>
       </c>
-      <c r="F17" s="56" t="s">
+      <c r="F17" s="57" t="s">
         <v>69</v>
       </c>
       <c r="G17" s="7" t="s">
@@ -3577,23 +3580,25 @@
       <c r="J17" s="2">
         <v>2026</v>
       </c>
-      <c r="K17" s="58">
-        <v>0</v>
-      </c>
-      <c r="L17" s="58" t="s">
+      <c r="K17" s="59">
+        <v>0</v>
+      </c>
+      <c r="L17" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="M17" s="58"/>
-      <c r="N17" s="59">
+      <c r="M17" s="59">
+        <v>0.25</v>
+      </c>
+      <c r="N17" s="60">
         <v>0.45</v>
       </c>
-      <c r="O17" s="59">
+      <c r="O17" s="60">
         <v>0.6</v>
       </c>
-      <c r="P17" s="61" t="s">
+      <c r="P17" s="62" t="s">
         <v>428</v>
       </c>
-      <c r="Q17" s="61" t="s">
+      <c r="Q17" s="62" t="s">
         <v>405</v>
       </c>
       <c r="R17" s="28" t="s">
@@ -3604,12 +3609,12 @@
       </c>
     </row>
     <row r="18" spans="1:20" ht="72" customHeight="1">
-      <c r="A18" s="57"/>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="71"/>
-      <c r="F18" s="57"/>
+      <c r="A18" s="58"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="58"/>
+      <c r="E18" s="72"/>
+      <c r="F18" s="58"/>
       <c r="G18" s="7" t="s">
         <v>386</v>
       </c>
@@ -3623,13 +3628,13 @@
       <c r="J18" s="2">
         <v>2030</v>
       </c>
-      <c r="K18" s="58"/>
-      <c r="L18" s="58"/>
-      <c r="M18" s="58"/>
-      <c r="N18" s="59"/>
-      <c r="O18" s="59"/>
-      <c r="P18" s="61"/>
-      <c r="Q18" s="61"/>
+      <c r="K18" s="59"/>
+      <c r="L18" s="59"/>
+      <c r="M18" s="59"/>
+      <c r="N18" s="60"/>
+      <c r="O18" s="60"/>
+      <c r="P18" s="62"/>
+      <c r="Q18" s="62"/>
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
     </row>
@@ -4497,9 +4502,7 @@
       </c>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
-      <c r="O35" s="16">
-        <v>0.5</v>
-      </c>
+      <c r="O35" s="16"/>
       <c r="P35" s="15"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="2"/>
@@ -4592,22 +4595,22 @@
       </c>
     </row>
     <row r="38" spans="1:19" ht="72" customHeight="1">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" s="28" t="s">
         <v>152</v>
       </c>
-      <c r="E38" s="27" t="s">
+      <c r="E38" s="56" t="s">
         <v>153</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F38" s="28" t="s">
         <v>154</v>
       </c>
       <c r="G38" s="7" t="s">
@@ -4629,9 +4632,7 @@
       <c r="L38" s="3">
         <v>1</v>
       </c>
-      <c r="M38" s="3">
-        <v>0.5</v>
-      </c>
+      <c r="M38" s="3"/>
       <c r="N38" s="3">
         <v>0.5</v>
       </c>
@@ -4652,22 +4653,22 @@
       </c>
     </row>
     <row r="39" spans="1:19" ht="72" customHeight="1">
-      <c r="A39" s="66" t="s">
+      <c r="A39" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="66" t="s">
+      <c r="B39" s="67" t="s">
         <v>155</v>
       </c>
-      <c r="C39" s="66" t="s">
+      <c r="C39" s="67" t="s">
         <v>156</v>
       </c>
-      <c r="D39" s="66" t="s">
+      <c r="D39" s="67" t="s">
         <v>157</v>
       </c>
-      <c r="E39" s="68" t="s">
+      <c r="E39" s="69" t="s">
         <v>158</v>
       </c>
-      <c r="F39" s="66" t="s">
+      <c r="F39" s="67" t="s">
         <v>159</v>
       </c>
       <c r="G39" s="2" t="s">
@@ -4683,25 +4684,25 @@
       <c r="J39" s="2">
         <v>2030</v>
       </c>
-      <c r="K39" s="58">
-        <v>0</v>
-      </c>
-      <c r="L39" s="58">
+      <c r="K39" s="59">
+        <v>0</v>
+      </c>
+      <c r="L39" s="59">
         <v>1</v>
       </c>
-      <c r="M39" s="62">
+      <c r="M39" s="63">
         <v>0.4</v>
       </c>
-      <c r="N39" s="58">
+      <c r="N39" s="59">
         <v>0.4</v>
       </c>
-      <c r="O39" s="59">
+      <c r="O39" s="60">
         <v>0.6</v>
       </c>
-      <c r="P39" s="76" t="s">
+      <c r="P39" s="77" t="s">
         <v>413</v>
       </c>
-      <c r="Q39" s="61" t="s">
+      <c r="Q39" s="62" t="s">
         <v>413</v>
       </c>
       <c r="R39" s="28" t="s">
@@ -4712,12 +4713,12 @@
       </c>
     </row>
     <row r="40" spans="1:19" ht="72" customHeight="1">
-      <c r="A40" s="67"/>
-      <c r="B40" s="67"/>
-      <c r="C40" s="67"/>
-      <c r="D40" s="67"/>
-      <c r="E40" s="69"/>
-      <c r="F40" s="67"/>
+      <c r="A40" s="68"/>
+      <c r="B40" s="68"/>
+      <c r="C40" s="68"/>
+      <c r="D40" s="68"/>
+      <c r="E40" s="70"/>
+      <c r="F40" s="68"/>
       <c r="G40" s="2" t="s">
         <v>161</v>
       </c>
@@ -4731,13 +4732,13 @@
       <c r="J40" s="2">
         <v>2030</v>
       </c>
-      <c r="K40" s="58"/>
-      <c r="L40" s="58"/>
-      <c r="M40" s="63"/>
-      <c r="N40" s="58"/>
-      <c r="O40" s="59"/>
-      <c r="P40" s="77"/>
-      <c r="Q40" s="61"/>
+      <c r="K40" s="59"/>
+      <c r="L40" s="59"/>
+      <c r="M40" s="64"/>
+      <c r="N40" s="59"/>
+      <c r="O40" s="60"/>
+      <c r="P40" s="78"/>
+      <c r="Q40" s="62"/>
       <c r="R40" s="28" t="s">
         <v>354</v>
       </c>
@@ -4806,22 +4807,22 @@
       </c>
     </row>
     <row r="42" spans="1:19" ht="72" customHeight="1">
-      <c r="A42" s="66" t="s">
+      <c r="A42" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="66" t="s">
+      <c r="B42" s="67" t="s">
         <v>155</v>
       </c>
-      <c r="C42" s="66" t="s">
+      <c r="C42" s="67" t="s">
         <v>166</v>
       </c>
-      <c r="D42" s="66" t="s">
+      <c r="D42" s="67" t="s">
         <v>167</v>
       </c>
-      <c r="E42" s="68" t="s">
+      <c r="E42" s="69" t="s">
         <v>168</v>
       </c>
-      <c r="F42" s="66" t="s">
+      <c r="F42" s="67" t="s">
         <v>169</v>
       </c>
       <c r="G42" s="7" t="s">
@@ -4837,25 +4838,25 @@
       <c r="J42" s="2">
         <v>2026</v>
       </c>
-      <c r="K42" s="58">
-        <v>0</v>
-      </c>
-      <c r="L42" s="58">
+      <c r="K42" s="59">
+        <v>0</v>
+      </c>
+      <c r="L42" s="59">
         <v>1</v>
       </c>
-      <c r="M42" s="58">
+      <c r="M42" s="59">
         <v>0.45</v>
       </c>
-      <c r="N42" s="58">
+      <c r="N42" s="59">
         <v>0.45</v>
       </c>
-      <c r="O42" s="59">
+      <c r="O42" s="60">
         <v>0.95</v>
       </c>
-      <c r="P42" s="61" t="s">
+      <c r="P42" s="62" t="s">
         <v>415</v>
       </c>
-      <c r="Q42" s="61" t="s">
+      <c r="Q42" s="62" t="s">
         <v>415</v>
       </c>
       <c r="R42" s="28" t="s">
@@ -4866,12 +4867,12 @@
       </c>
     </row>
     <row r="43" spans="1:19" ht="72" customHeight="1">
-      <c r="A43" s="67"/>
-      <c r="B43" s="67"/>
-      <c r="C43" s="67"/>
-      <c r="D43" s="67"/>
-      <c r="E43" s="69"/>
-      <c r="F43" s="67"/>
+      <c r="A43" s="68"/>
+      <c r="B43" s="68"/>
+      <c r="C43" s="68"/>
+      <c r="D43" s="68"/>
+      <c r="E43" s="70"/>
+      <c r="F43" s="68"/>
       <c r="G43" s="2" t="s">
         <v>170</v>
       </c>
@@ -4885,13 +4886,13 @@
       <c r="J43" s="2">
         <v>2030</v>
       </c>
-      <c r="K43" s="58"/>
-      <c r="L43" s="58"/>
-      <c r="M43" s="58"/>
-      <c r="N43" s="58"/>
-      <c r="O43" s="59"/>
-      <c r="P43" s="61"/>
-      <c r="Q43" s="61"/>
+      <c r="K43" s="59"/>
+      <c r="L43" s="59"/>
+      <c r="M43" s="59"/>
+      <c r="N43" s="59"/>
+      <c r="O43" s="60"/>
+      <c r="P43" s="62"/>
+      <c r="Q43" s="62"/>
       <c r="R43" s="2"/>
       <c r="S43" s="2"/>
     </row>
@@ -5059,16 +5060,16 @@
     <row r="47" spans="1:19" ht="72" customHeight="1">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
-      <c r="C47" s="66" t="s">
+      <c r="C47" s="67" t="s">
         <v>187</v>
       </c>
-      <c r="D47" s="66" t="s">
+      <c r="D47" s="67" t="s">
         <v>188</v>
       </c>
-      <c r="E47" s="68" t="s">
+      <c r="E47" s="69" t="s">
         <v>189</v>
       </c>
-      <c r="F47" s="66" t="s">
+      <c r="F47" s="67" t="s">
         <v>190</v>
       </c>
       <c r="G47" s="2" t="s">
@@ -5084,25 +5085,25 @@
       <c r="J47" s="2">
         <v>2030</v>
       </c>
-      <c r="K47" s="58">
-        <v>0</v>
-      </c>
-      <c r="L47" s="58">
+      <c r="K47" s="59">
+        <v>0</v>
+      </c>
+      <c r="L47" s="59">
         <v>1</v>
       </c>
-      <c r="M47" s="58">
+      <c r="M47" s="59">
         <v>0.5</v>
       </c>
-      <c r="N47" s="58">
+      <c r="N47" s="59">
         <v>0.5</v>
       </c>
-      <c r="O47" s="59">
+      <c r="O47" s="60">
         <v>0.7</v>
       </c>
-      <c r="P47" s="60" t="s">
+      <c r="P47" s="61" t="s">
         <v>418</v>
       </c>
-      <c r="Q47" s="60" t="s">
+      <c r="Q47" s="61" t="s">
         <v>418</v>
       </c>
       <c r="R47" s="28" t="s">
@@ -5119,10 +5120,10 @@
       <c r="B48" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C48" s="67"/>
-      <c r="D48" s="67"/>
-      <c r="E48" s="69"/>
-      <c r="F48" s="67"/>
+      <c r="C48" s="68"/>
+      <c r="D48" s="68"/>
+      <c r="E48" s="70"/>
+      <c r="F48" s="68"/>
       <c r="G48" s="2" t="s">
         <v>204</v>
       </c>
@@ -5136,33 +5137,33 @@
       <c r="J48" s="2">
         <v>2030</v>
       </c>
-      <c r="K48" s="58"/>
-      <c r="L48" s="58"/>
-      <c r="M48" s="58"/>
-      <c r="N48" s="58"/>
-      <c r="O48" s="59"/>
-      <c r="P48" s="60"/>
-      <c r="Q48" s="60"/>
+      <c r="K48" s="59"/>
+      <c r="L48" s="59"/>
+      <c r="M48" s="59"/>
+      <c r="N48" s="59"/>
+      <c r="O48" s="60"/>
+      <c r="P48" s="61"/>
+      <c r="Q48" s="61"/>
       <c r="R48" s="2"/>
       <c r="S48" s="2"/>
     </row>
     <row r="49" spans="1:20" ht="72" customHeight="1">
-      <c r="A49" s="66" t="s">
+      <c r="A49" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="66" t="s">
+      <c r="B49" s="67" t="s">
         <v>186</v>
       </c>
-      <c r="C49" s="66" t="s">
+      <c r="C49" s="67" t="s">
         <v>192</v>
       </c>
-      <c r="D49" s="66" t="s">
+      <c r="D49" s="67" t="s">
         <v>193</v>
       </c>
-      <c r="E49" s="68" t="s">
+      <c r="E49" s="69" t="s">
         <v>194</v>
       </c>
-      <c r="F49" s="66" t="s">
+      <c r="F49" s="67" t="s">
         <v>195</v>
       </c>
       <c r="G49" s="7" t="s">
@@ -5178,25 +5179,25 @@
       <c r="J49" s="2">
         <v>2030</v>
       </c>
-      <c r="K49" s="58">
-        <v>0</v>
-      </c>
-      <c r="L49" s="58">
+      <c r="K49" s="59">
+        <v>0</v>
+      </c>
+      <c r="L49" s="59">
         <v>1</v>
       </c>
-      <c r="M49" s="58">
+      <c r="M49" s="59">
         <v>0.5</v>
       </c>
-      <c r="N49" s="58">
+      <c r="N49" s="59">
         <v>0.5</v>
       </c>
-      <c r="O49" s="59">
+      <c r="O49" s="60">
         <v>0.7</v>
       </c>
-      <c r="P49" s="60" t="s">
+      <c r="P49" s="61" t="s">
         <v>418</v>
       </c>
-      <c r="Q49" s="60" t="s">
+      <c r="Q49" s="61" t="s">
         <v>418</v>
       </c>
       <c r="R49" s="28" t="s">
@@ -5207,12 +5208,12 @@
       </c>
     </row>
     <row r="50" spans="1:20" ht="72" customHeight="1">
-      <c r="A50" s="74"/>
-      <c r="B50" s="74"/>
-      <c r="C50" s="74"/>
-      <c r="D50" s="74"/>
-      <c r="E50" s="75"/>
-      <c r="F50" s="74"/>
+      <c r="A50" s="75"/>
+      <c r="B50" s="75"/>
+      <c r="C50" s="75"/>
+      <c r="D50" s="75"/>
+      <c r="E50" s="76"/>
+      <c r="F50" s="75"/>
       <c r="G50" s="7" t="s">
         <v>204</v>
       </c>
@@ -5226,13 +5227,13 @@
       <c r="J50" s="2">
         <v>2030</v>
       </c>
-      <c r="K50" s="58"/>
-      <c r="L50" s="58"/>
-      <c r="M50" s="58"/>
-      <c r="N50" s="58"/>
-      <c r="O50" s="59"/>
-      <c r="P50" s="60"/>
-      <c r="Q50" s="60"/>
+      <c r="K50" s="59"/>
+      <c r="L50" s="59"/>
+      <c r="M50" s="59"/>
+      <c r="N50" s="59"/>
+      <c r="O50" s="60"/>
+      <c r="P50" s="61"/>
+      <c r="Q50" s="61"/>
       <c r="R50" s="28" t="s">
         <v>368</v>
       </c>
@@ -5421,22 +5422,22 @@
       </c>
     </row>
     <row r="54" spans="1:20" ht="72" customHeight="1">
-      <c r="A54" s="66" t="s">
+      <c r="A54" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="B54" s="66" t="s">
+      <c r="B54" s="67" t="s">
         <v>186</v>
       </c>
-      <c r="C54" s="66" t="s">
+      <c r="C54" s="67" t="s">
         <v>210</v>
       </c>
-      <c r="D54" s="66" t="s">
+      <c r="D54" s="67" t="s">
         <v>211</v>
       </c>
-      <c r="E54" s="68" t="s">
+      <c r="E54" s="69" t="s">
         <v>212</v>
       </c>
-      <c r="F54" s="66" t="s">
+      <c r="F54" s="67" t="s">
         <v>213</v>
       </c>
       <c r="G54" s="2" t="s">
@@ -5452,25 +5453,25 @@
       <c r="J54" s="2">
         <v>2030</v>
       </c>
-      <c r="K54" s="58">
-        <v>0</v>
-      </c>
-      <c r="L54" s="58">
+      <c r="K54" s="59">
+        <v>0</v>
+      </c>
+      <c r="L54" s="59">
         <v>1</v>
       </c>
-      <c r="M54" s="62">
+      <c r="M54" s="63">
         <v>0.5</v>
       </c>
-      <c r="N54" s="58">
+      <c r="N54" s="59">
         <v>0.5</v>
       </c>
-      <c r="O54" s="59">
+      <c r="O54" s="60">
         <v>0.7</v>
       </c>
-      <c r="P54" s="60" t="s">
+      <c r="P54" s="61" t="s">
         <v>418</v>
       </c>
-      <c r="Q54" s="60" t="s">
+      <c r="Q54" s="61" t="s">
         <v>418</v>
       </c>
       <c r="R54" s="28" t="s">
@@ -5481,12 +5482,12 @@
       </c>
     </row>
     <row r="55" spans="1:20" ht="72" customHeight="1">
-      <c r="A55" s="67"/>
-      <c r="B55" s="67"/>
-      <c r="C55" s="67"/>
-      <c r="D55" s="67"/>
-      <c r="E55" s="69"/>
-      <c r="F55" s="67"/>
+      <c r="A55" s="68"/>
+      <c r="B55" s="68"/>
+      <c r="C55" s="68"/>
+      <c r="D55" s="68"/>
+      <c r="E55" s="70"/>
+      <c r="F55" s="68"/>
       <c r="G55" s="2" t="s">
         <v>204</v>
       </c>
@@ -5500,13 +5501,13 @@
       <c r="J55" s="2">
         <v>2030</v>
       </c>
-      <c r="K55" s="58"/>
-      <c r="L55" s="58"/>
-      <c r="M55" s="63"/>
-      <c r="N55" s="58"/>
-      <c r="O55" s="59"/>
-      <c r="P55" s="60"/>
-      <c r="Q55" s="60"/>
+      <c r="K55" s="59"/>
+      <c r="L55" s="59"/>
+      <c r="M55" s="64"/>
+      <c r="N55" s="59"/>
+      <c r="O55" s="60"/>
+      <c r="P55" s="61"/>
+      <c r="Q55" s="61"/>
       <c r="R55" s="28" t="s">
         <v>368</v>
       </c>
@@ -6074,7 +6075,9 @@
       <c r="N66" s="3">
         <v>0.5</v>
       </c>
-      <c r="O66" s="16"/>
+      <c r="O66" s="16">
+        <v>1</v>
+      </c>
       <c r="P66" s="15"/>
       <c r="Q66" s="7"/>
       <c r="R66" s="2"/>
@@ -7868,7 +7871,7 @@
   <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -7955,9 +7958,9 @@
         <f>IF(VLOOKUP(D3,main!C:O,12,FALSE)=0,"",VLOOKUP(D3,main!C:O,12,FALSE))</f>
         <v/>
       </c>
-      <c r="G3" s="21">
+      <c r="G3" s="21" t="str">
         <f>IF(VLOOKUP(D3,main!C:O,13,FALSE)=0,"",VLOOKUP(D3,main!C:O,13,FALSE))</f>
-        <v>0.5</v>
+        <v/>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -8207,9 +8210,9 @@
       <c r="D13" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="21" t="str">
+      <c r="E13" s="21">
         <f>IF(VLOOKUP(D13,main!C:O,11,FALSE)=0,"",VLOOKUP(D13,main!C:O,11,FALSE))</f>
-        <v/>
+        <v>0.25</v>
       </c>
       <c r="F13" s="21">
         <f>IF(VLOOKUP(D13,main!C:O,12,FALSE)=0,"",VLOOKUP(D13,main!C:O,12,FALSE))</f>
@@ -8233,9 +8236,9 @@
       <c r="D14" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="21" t="str">
+      <c r="E14" s="21">
         <f>IF(VLOOKUP(D14,main!C:O,11,FALSE)=0,"",VLOOKUP(D14,main!C:O,11,FALSE))</f>
-        <v/>
+        <v>0.25</v>
       </c>
       <c r="F14" s="21">
         <f>IF(VLOOKUP(D14,main!C:O,12,FALSE)=0,"",VLOOKUP(D14,main!C:O,12,FALSE))</f>
@@ -8683,9 +8686,9 @@
         <f>IF(VLOOKUP(D31,main!C:O,12,FALSE)=0,"",VLOOKUP(D31,main!C:O,12,FALSE))</f>
         <v/>
       </c>
-      <c r="G31" s="21">
+      <c r="G31" s="21" t="str">
         <f>IF(VLOOKUP(D31,main!C:O,13,FALSE)=0,"",VLOOKUP(D31,main!C:O,13,FALSE))</f>
-        <v>0.5</v>
+        <v/>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -8753,9 +8756,9 @@
       <c r="D34" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="21" t="str">
         <f>IF(VLOOKUP(D34,main!C:O,11,FALSE)=0,"",VLOOKUP(D34,main!C:O,11,FALSE))</f>
-        <v>0.5</v>
+        <v/>
       </c>
       <c r="F34" s="21">
         <f>IF(VLOOKUP(D34,main!C:O,12,FALSE)=0,"",VLOOKUP(D34,main!C:O,12,FALSE))</f>
@@ -9359,9 +9362,9 @@
         <f>IF(VLOOKUP(D57,main!C:O,12,FALSE)=0,"",VLOOKUP(D57,main!C:O,12,FALSE))</f>
         <v>0.5</v>
       </c>
-      <c r="G57" s="21" t="str">
+      <c r="G57" s="21">
         <f>IF(VLOOKUP(D57,main!C:O,13,FALSE)=0,"",VLOOKUP(D57,main!C:O,13,FALSE))</f>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:7">

</xml_diff>

<commit_message>
large update of waso transformations
</commit_message>
<xml_diff>
--- a/croatia/data/ssp_croatia_transformation_2024_12_13_testing_ver.xlsx
+++ b/croatia/data/ssp_croatia_transformation_2024_12_13_testing_ver.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarob\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D74EE1E-0633-4894-B59E-4ECD7385C4F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA210DDB-A8FE-4B28-8CFF-498859322943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2234,7 +2234,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2373,6 +2373,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2412,18 +2418,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2435,6 +2429,30 @@
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2744,9 +2762,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1048523"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M4" sqref="M4"/>
+      <selection pane="topRight" activeCell="M71" sqref="M71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -2980,22 +2998,22 @@
       </c>
     </row>
     <row r="5" spans="1:20" ht="143.44999999999999" customHeight="1">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="67" t="s">
+      <c r="C5" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="67" t="s">
+      <c r="D5" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="69" t="s">
+      <c r="E5" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="67" t="s">
+      <c r="F5" s="69" t="s">
         <v>26</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -3011,37 +3029,37 @@
       <c r="J5" s="2">
         <v>2030</v>
       </c>
-      <c r="K5" s="59">
-        <v>0</v>
-      </c>
-      <c r="L5" s="59">
+      <c r="K5" s="61">
+        <v>0</v>
+      </c>
+      <c r="L5" s="61">
         <v>1</v>
       </c>
-      <c r="M5" s="59">
+      <c r="M5" s="61">
         <v>0.4</v>
       </c>
-      <c r="N5" s="59">
+      <c r="N5" s="61">
         <v>0.4</v>
       </c>
-      <c r="O5" s="60">
+      <c r="O5" s="62">
         <v>0.95</v>
       </c>
-      <c r="P5" s="62" t="s">
+      <c r="P5" s="64" t="s">
         <v>403</v>
       </c>
-      <c r="Q5" s="62" t="s">
+      <c r="Q5" s="64" t="s">
         <v>403</v>
       </c>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
     </row>
     <row r="6" spans="1:20" ht="72" customHeight="1">
-      <c r="A6" s="68"/>
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="68"/>
+      <c r="A6" s="70"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="70"/>
       <c r="G6" s="7" t="s">
         <v>388</v>
       </c>
@@ -3055,13 +3073,13 @@
       <c r="J6" s="2">
         <v>2030</v>
       </c>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
-      <c r="M6" s="59"/>
-      <c r="N6" s="59"/>
-      <c r="O6" s="60"/>
-      <c r="P6" s="62"/>
-      <c r="Q6" s="62"/>
+      <c r="K6" s="61"/>
+      <c r="L6" s="61"/>
+      <c r="M6" s="61"/>
+      <c r="N6" s="61"/>
+      <c r="O6" s="62"/>
+      <c r="P6" s="64"/>
+      <c r="Q6" s="64"/>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
     </row>
@@ -3163,22 +3181,22 @@
       </c>
     </row>
     <row r="9" spans="1:20" ht="72" customHeight="1">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="67" t="s">
+      <c r="C9" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="67" t="s">
+      <c r="D9" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="69" t="s">
+      <c r="E9" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="67" t="s">
+      <c r="F9" s="69" t="s">
         <v>42</v>
       </c>
       <c r="G9" s="7" t="s">
@@ -3194,28 +3212,28 @@
       <c r="J9" s="2">
         <v>2030</v>
       </c>
-      <c r="K9" s="59">
-        <v>0</v>
-      </c>
-      <c r="L9" s="59">
+      <c r="K9" s="61">
+        <v>0</v>
+      </c>
+      <c r="L9" s="61">
         <v>1</v>
       </c>
-      <c r="M9" s="59">
+      <c r="M9" s="61">
         <v>0.3</v>
       </c>
-      <c r="N9" s="59">
+      <c r="N9" s="61">
         <v>0.3</v>
       </c>
-      <c r="O9" s="60">
+      <c r="O9" s="62">
         <v>0.6</v>
       </c>
-      <c r="P9" s="62" t="s">
+      <c r="P9" s="64" t="s">
         <v>427</v>
       </c>
-      <c r="Q9" s="62" t="s">
+      <c r="Q9" s="64" t="s">
         <v>427</v>
       </c>
-      <c r="R9" s="57" t="s">
+      <c r="R9" s="59" t="s">
         <v>353</v>
       </c>
       <c r="S9" s="2" t="s">
@@ -3223,12 +3241,12 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="72" customHeight="1">
-      <c r="A10" s="68"/>
-      <c r="B10" s="68"/>
-      <c r="C10" s="68"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="70"/>
-      <c r="F10" s="68"/>
+      <c r="A10" s="70"/>
+      <c r="B10" s="70"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="70"/>
       <c r="G10" s="2" t="s">
         <v>43</v>
       </c>
@@ -3242,14 +3260,14 @@
       <c r="J10" s="2">
         <v>2030</v>
       </c>
-      <c r="K10" s="59"/>
-      <c r="L10" s="59"/>
-      <c r="M10" s="59"/>
-      <c r="N10" s="59"/>
-      <c r="O10" s="60"/>
-      <c r="P10" s="62"/>
-      <c r="Q10" s="62"/>
-      <c r="R10" s="58"/>
+      <c r="K10" s="61"/>
+      <c r="L10" s="61"/>
+      <c r="M10" s="61"/>
+      <c r="N10" s="61"/>
+      <c r="O10" s="62"/>
+      <c r="P10" s="64"/>
+      <c r="Q10" s="64"/>
+      <c r="R10" s="60"/>
       <c r="S10" s="2" t="s">
         <v>645</v>
       </c>
@@ -3459,22 +3477,22 @@
       </c>
     </row>
     <row r="15" spans="1:20" ht="72" customHeight="1">
-      <c r="A15" s="73" t="s">
+      <c r="A15" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="73" t="s">
+      <c r="B15" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="73" t="s">
+      <c r="C15" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="73" t="s">
+      <c r="D15" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="E15" s="74" t="s">
+      <c r="E15" s="78" t="s">
         <v>64</v>
       </c>
-      <c r="F15" s="73" t="s">
+      <c r="F15" s="77" t="s">
         <v>65</v>
       </c>
       <c r="G15" s="7" t="s">
@@ -3490,25 +3508,25 @@
       <c r="J15" s="2">
         <v>2026</v>
       </c>
-      <c r="K15" s="59">
-        <v>0</v>
-      </c>
-      <c r="L15" s="59" t="s">
+      <c r="K15" s="61">
+        <v>0</v>
+      </c>
+      <c r="L15" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="M15" s="59">
+      <c r="M15" s="61">
         <v>0.25</v>
       </c>
-      <c r="N15" s="60">
+      <c r="N15" s="62">
         <v>0.45</v>
       </c>
-      <c r="O15" s="60">
+      <c r="O15" s="62">
         <v>0.6</v>
       </c>
-      <c r="P15" s="62" t="s">
+      <c r="P15" s="64" t="s">
         <v>428</v>
       </c>
-      <c r="Q15" s="65" t="s">
+      <c r="Q15" s="67" t="s">
         <v>405</v>
       </c>
       <c r="R15" s="28" t="s">
@@ -3519,12 +3537,12 @@
       </c>
     </row>
     <row r="16" spans="1:20" ht="72" customHeight="1">
-      <c r="A16" s="73"/>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="74"/>
-      <c r="F16" s="73"/>
+      <c r="A16" s="77"/>
+      <c r="B16" s="77"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="77"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="77"/>
       <c r="G16" s="7" t="s">
         <v>386</v>
       </c>
@@ -3538,33 +3556,33 @@
       <c r="J16" s="2">
         <v>2030</v>
       </c>
-      <c r="K16" s="59"/>
-      <c r="L16" s="59"/>
-      <c r="M16" s="59"/>
-      <c r="N16" s="60"/>
-      <c r="O16" s="60"/>
-      <c r="P16" s="62"/>
-      <c r="Q16" s="66"/>
+      <c r="K16" s="61"/>
+      <c r="L16" s="61"/>
+      <c r="M16" s="61"/>
+      <c r="N16" s="62"/>
+      <c r="O16" s="62"/>
+      <c r="P16" s="64"/>
+      <c r="Q16" s="68"/>
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
     </row>
     <row r="17" spans="1:20" ht="72" customHeight="1">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="57" t="s">
+      <c r="B17" s="79" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="57" t="s">
+      <c r="C17" s="79" t="s">
         <v>66</v>
       </c>
-      <c r="D17" s="57" t="s">
+      <c r="D17" s="79" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="71" t="s">
+      <c r="E17" s="80" t="s">
         <v>68</v>
       </c>
-      <c r="F17" s="57" t="s">
+      <c r="F17" s="79" t="s">
         <v>69</v>
       </c>
       <c r="G17" s="7" t="s">
@@ -3580,25 +3598,25 @@
       <c r="J17" s="2">
         <v>2026</v>
       </c>
-      <c r="K17" s="59">
-        <v>0</v>
-      </c>
-      <c r="L17" s="59" t="s">
+      <c r="K17" s="61">
+        <v>0</v>
+      </c>
+      <c r="L17" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="M17" s="59">
+      <c r="M17" s="61">
         <v>0.25</v>
       </c>
-      <c r="N17" s="60">
+      <c r="N17" s="62">
         <v>0.45</v>
       </c>
-      <c r="O17" s="60">
+      <c r="O17" s="62">
         <v>0.6</v>
       </c>
-      <c r="P17" s="62" t="s">
+      <c r="P17" s="64" t="s">
         <v>428</v>
       </c>
-      <c r="Q17" s="62" t="s">
+      <c r="Q17" s="64" t="s">
         <v>405</v>
       </c>
       <c r="R17" s="28" t="s">
@@ -3609,12 +3627,12 @@
       </c>
     </row>
     <row r="18" spans="1:20" ht="72" customHeight="1">
-      <c r="A18" s="58"/>
-      <c r="B18" s="58"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="72"/>
-      <c r="F18" s="58"/>
+      <c r="A18" s="81"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="81"/>
+      <c r="D18" s="81"/>
+      <c r="E18" s="82"/>
+      <c r="F18" s="81"/>
       <c r="G18" s="7" t="s">
         <v>386</v>
       </c>
@@ -3628,13 +3646,13 @@
       <c r="J18" s="2">
         <v>2030</v>
       </c>
-      <c r="K18" s="59"/>
-      <c r="L18" s="59"/>
-      <c r="M18" s="59"/>
-      <c r="N18" s="60"/>
-      <c r="O18" s="60"/>
-      <c r="P18" s="62"/>
-      <c r="Q18" s="62"/>
+      <c r="K18" s="61"/>
+      <c r="L18" s="61"/>
+      <c r="M18" s="61"/>
+      <c r="N18" s="62"/>
+      <c r="O18" s="62"/>
+      <c r="P18" s="64"/>
+      <c r="Q18" s="64"/>
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
     </row>
@@ -4633,9 +4651,7 @@
         <v>1</v>
       </c>
       <c r="M38" s="3"/>
-      <c r="N38" s="3">
-        <v>0.5</v>
-      </c>
+      <c r="N38" s="3"/>
       <c r="O38" s="16">
         <v>0.8</v>
       </c>
@@ -4653,22 +4669,22 @@
       </c>
     </row>
     <row r="39" spans="1:19" ht="72" customHeight="1">
-      <c r="A39" s="67" t="s">
+      <c r="A39" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="67" t="s">
+      <c r="B39" s="69" t="s">
         <v>155</v>
       </c>
-      <c r="C39" s="67" t="s">
+      <c r="C39" s="69" t="s">
         <v>156</v>
       </c>
-      <c r="D39" s="67" t="s">
+      <c r="D39" s="69" t="s">
         <v>157</v>
       </c>
-      <c r="E39" s="69" t="s">
+      <c r="E39" s="71" t="s">
         <v>158</v>
       </c>
-      <c r="F39" s="67" t="s">
+      <c r="F39" s="69" t="s">
         <v>159</v>
       </c>
       <c r="G39" s="2" t="s">
@@ -4684,25 +4700,25 @@
       <c r="J39" s="2">
         <v>2030</v>
       </c>
-      <c r="K39" s="59">
-        <v>0</v>
-      </c>
-      <c r="L39" s="59">
+      <c r="K39" s="61">
+        <v>0</v>
+      </c>
+      <c r="L39" s="61">
         <v>1</v>
       </c>
-      <c r="M39" s="63">
+      <c r="M39" s="65">
         <v>0.4</v>
       </c>
-      <c r="N39" s="59">
+      <c r="N39" s="61">
         <v>0.4</v>
       </c>
-      <c r="O39" s="60">
+      <c r="O39" s="62">
         <v>0.6</v>
       </c>
-      <c r="P39" s="77" t="s">
+      <c r="P39" s="75" t="s">
         <v>413</v>
       </c>
-      <c r="Q39" s="62" t="s">
+      <c r="Q39" s="64" t="s">
         <v>413</v>
       </c>
       <c r="R39" s="28" t="s">
@@ -4713,12 +4729,12 @@
       </c>
     </row>
     <row r="40" spans="1:19" ht="72" customHeight="1">
-      <c r="A40" s="68"/>
-      <c r="B40" s="68"/>
-      <c r="C40" s="68"/>
-      <c r="D40" s="68"/>
-      <c r="E40" s="70"/>
-      <c r="F40" s="68"/>
+      <c r="A40" s="70"/>
+      <c r="B40" s="70"/>
+      <c r="C40" s="70"/>
+      <c r="D40" s="70"/>
+      <c r="E40" s="72"/>
+      <c r="F40" s="70"/>
       <c r="G40" s="2" t="s">
         <v>161</v>
       </c>
@@ -4732,13 +4748,13 @@
       <c r="J40" s="2">
         <v>2030</v>
       </c>
-      <c r="K40" s="59"/>
-      <c r="L40" s="59"/>
-      <c r="M40" s="64"/>
-      <c r="N40" s="59"/>
-      <c r="O40" s="60"/>
-      <c r="P40" s="78"/>
-      <c r="Q40" s="62"/>
+      <c r="K40" s="61"/>
+      <c r="L40" s="61"/>
+      <c r="M40" s="66"/>
+      <c r="N40" s="61"/>
+      <c r="O40" s="62"/>
+      <c r="P40" s="76"/>
+      <c r="Q40" s="64"/>
       <c r="R40" s="28" t="s">
         <v>354</v>
       </c>
@@ -4807,22 +4823,22 @@
       </c>
     </row>
     <row r="42" spans="1:19" ht="72" customHeight="1">
-      <c r="A42" s="67" t="s">
+      <c r="A42" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="67" t="s">
+      <c r="B42" s="69" t="s">
         <v>155</v>
       </c>
-      <c r="C42" s="67" t="s">
+      <c r="C42" s="69" t="s">
         <v>166</v>
       </c>
-      <c r="D42" s="67" t="s">
+      <c r="D42" s="69" t="s">
         <v>167</v>
       </c>
-      <c r="E42" s="69" t="s">
+      <c r="E42" s="71" t="s">
         <v>168</v>
       </c>
-      <c r="F42" s="67" t="s">
+      <c r="F42" s="69" t="s">
         <v>169</v>
       </c>
       <c r="G42" s="7" t="s">
@@ -4838,25 +4854,25 @@
       <c r="J42" s="2">
         <v>2026</v>
       </c>
-      <c r="K42" s="59">
-        <v>0</v>
-      </c>
-      <c r="L42" s="59">
+      <c r="K42" s="61">
+        <v>0</v>
+      </c>
+      <c r="L42" s="61">
         <v>1</v>
       </c>
-      <c r="M42" s="59">
+      <c r="M42" s="61">
         <v>0.45</v>
       </c>
-      <c r="N42" s="59">
+      <c r="N42" s="61">
         <v>0.45</v>
       </c>
-      <c r="O42" s="60">
+      <c r="O42" s="62">
         <v>0.95</v>
       </c>
-      <c r="P42" s="62" t="s">
+      <c r="P42" s="64" t="s">
         <v>415</v>
       </c>
-      <c r="Q42" s="62" t="s">
+      <c r="Q42" s="64" t="s">
         <v>415</v>
       </c>
       <c r="R42" s="28" t="s">
@@ -4867,12 +4883,12 @@
       </c>
     </row>
     <row r="43" spans="1:19" ht="72" customHeight="1">
-      <c r="A43" s="68"/>
-      <c r="B43" s="68"/>
-      <c r="C43" s="68"/>
-      <c r="D43" s="68"/>
-      <c r="E43" s="70"/>
-      <c r="F43" s="68"/>
+      <c r="A43" s="70"/>
+      <c r="B43" s="70"/>
+      <c r="C43" s="70"/>
+      <c r="D43" s="70"/>
+      <c r="E43" s="72"/>
+      <c r="F43" s="70"/>
       <c r="G43" s="2" t="s">
         <v>170</v>
       </c>
@@ -4886,13 +4902,13 @@
       <c r="J43" s="2">
         <v>2030</v>
       </c>
-      <c r="K43" s="59"/>
-      <c r="L43" s="59"/>
-      <c r="M43" s="59"/>
-      <c r="N43" s="59"/>
-      <c r="O43" s="60"/>
-      <c r="P43" s="62"/>
-      <c r="Q43" s="62"/>
+      <c r="K43" s="61"/>
+      <c r="L43" s="61"/>
+      <c r="M43" s="61"/>
+      <c r="N43" s="61"/>
+      <c r="O43" s="62"/>
+      <c r="P43" s="64"/>
+      <c r="Q43" s="64"/>
       <c r="R43" s="2"/>
       <c r="S43" s="2"/>
     </row>
@@ -5060,16 +5076,16 @@
     <row r="47" spans="1:19" ht="72" customHeight="1">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
-      <c r="C47" s="67" t="s">
+      <c r="C47" s="69" t="s">
         <v>187</v>
       </c>
-      <c r="D47" s="67" t="s">
+      <c r="D47" s="69" t="s">
         <v>188</v>
       </c>
-      <c r="E47" s="69" t="s">
+      <c r="E47" s="71" t="s">
         <v>189</v>
       </c>
-      <c r="F47" s="67" t="s">
+      <c r="F47" s="69" t="s">
         <v>190</v>
       </c>
       <c r="G47" s="2" t="s">
@@ -5085,25 +5101,25 @@
       <c r="J47" s="2">
         <v>2030</v>
       </c>
-      <c r="K47" s="59">
-        <v>0</v>
-      </c>
-      <c r="L47" s="59">
+      <c r="K47" s="61">
+        <v>0</v>
+      </c>
+      <c r="L47" s="61">
         <v>1</v>
       </c>
-      <c r="M47" s="59">
+      <c r="M47" s="61">
         <v>0.5</v>
       </c>
-      <c r="N47" s="59">
+      <c r="N47" s="61">
         <v>0.5</v>
       </c>
-      <c r="O47" s="60">
+      <c r="O47" s="62">
         <v>0.7</v>
       </c>
-      <c r="P47" s="61" t="s">
+      <c r="P47" s="63" t="s">
         <v>418</v>
       </c>
-      <c r="Q47" s="61" t="s">
+      <c r="Q47" s="63" t="s">
         <v>418</v>
       </c>
       <c r="R47" s="28" t="s">
@@ -5120,10 +5136,10 @@
       <c r="B48" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C48" s="68"/>
-      <c r="D48" s="68"/>
-      <c r="E48" s="70"/>
-      <c r="F48" s="68"/>
+      <c r="C48" s="70"/>
+      <c r="D48" s="70"/>
+      <c r="E48" s="72"/>
+      <c r="F48" s="70"/>
       <c r="G48" s="2" t="s">
         <v>204</v>
       </c>
@@ -5137,33 +5153,33 @@
       <c r="J48" s="2">
         <v>2030</v>
       </c>
-      <c r="K48" s="59"/>
-      <c r="L48" s="59"/>
-      <c r="M48" s="59"/>
-      <c r="N48" s="59"/>
-      <c r="O48" s="60"/>
-      <c r="P48" s="61"/>
-      <c r="Q48" s="61"/>
+      <c r="K48" s="61"/>
+      <c r="L48" s="61"/>
+      <c r="M48" s="61"/>
+      <c r="N48" s="61"/>
+      <c r="O48" s="62"/>
+      <c r="P48" s="63"/>
+      <c r="Q48" s="63"/>
       <c r="R48" s="2"/>
       <c r="S48" s="2"/>
     </row>
     <row r="49" spans="1:20" ht="72" customHeight="1">
-      <c r="A49" s="67" t="s">
+      <c r="A49" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="67" t="s">
+      <c r="B49" s="69" t="s">
         <v>186</v>
       </c>
-      <c r="C49" s="67" t="s">
+      <c r="C49" s="69" t="s">
         <v>192</v>
       </c>
-      <c r="D49" s="67" t="s">
+      <c r="D49" s="69" t="s">
         <v>193</v>
       </c>
-      <c r="E49" s="69" t="s">
+      <c r="E49" s="71" t="s">
         <v>194</v>
       </c>
-      <c r="F49" s="67" t="s">
+      <c r="F49" s="69" t="s">
         <v>195</v>
       </c>
       <c r="G49" s="7" t="s">
@@ -5179,25 +5195,25 @@
       <c r="J49" s="2">
         <v>2030</v>
       </c>
-      <c r="K49" s="59">
-        <v>0</v>
-      </c>
-      <c r="L49" s="59">
+      <c r="K49" s="61">
+        <v>0</v>
+      </c>
+      <c r="L49" s="61">
         <v>1</v>
       </c>
-      <c r="M49" s="59">
+      <c r="M49" s="61">
         <v>0.5</v>
       </c>
-      <c r="N49" s="59">
+      <c r="N49" s="61">
         <v>0.5</v>
       </c>
-      <c r="O49" s="60">
+      <c r="O49" s="62">
         <v>0.7</v>
       </c>
-      <c r="P49" s="61" t="s">
+      <c r="P49" s="63" t="s">
         <v>418</v>
       </c>
-      <c r="Q49" s="61" t="s">
+      <c r="Q49" s="63" t="s">
         <v>418</v>
       </c>
       <c r="R49" s="28" t="s">
@@ -5208,12 +5224,12 @@
       </c>
     </row>
     <row r="50" spans="1:20" ht="72" customHeight="1">
-      <c r="A50" s="75"/>
-      <c r="B50" s="75"/>
-      <c r="C50" s="75"/>
-      <c r="D50" s="75"/>
-      <c r="E50" s="76"/>
-      <c r="F50" s="75"/>
+      <c r="A50" s="73"/>
+      <c r="B50" s="73"/>
+      <c r="C50" s="73"/>
+      <c r="D50" s="73"/>
+      <c r="E50" s="74"/>
+      <c r="F50" s="73"/>
       <c r="G50" s="7" t="s">
         <v>204</v>
       </c>
@@ -5227,13 +5243,13 @@
       <c r="J50" s="2">
         <v>2030</v>
       </c>
-      <c r="K50" s="59"/>
-      <c r="L50" s="59"/>
-      <c r="M50" s="59"/>
-      <c r="N50" s="59"/>
-      <c r="O50" s="60"/>
-      <c r="P50" s="61"/>
-      <c r="Q50" s="61"/>
+      <c r="K50" s="61"/>
+      <c r="L50" s="61"/>
+      <c r="M50" s="61"/>
+      <c r="N50" s="61"/>
+      <c r="O50" s="62"/>
+      <c r="P50" s="63"/>
+      <c r="Q50" s="63"/>
       <c r="R50" s="28" t="s">
         <v>368</v>
       </c>
@@ -5422,22 +5438,22 @@
       </c>
     </row>
     <row r="54" spans="1:20" ht="72" customHeight="1">
-      <c r="A54" s="67" t="s">
+      <c r="A54" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="B54" s="67" t="s">
+      <c r="B54" s="69" t="s">
         <v>186</v>
       </c>
-      <c r="C54" s="67" t="s">
+      <c r="C54" s="69" t="s">
         <v>210</v>
       </c>
-      <c r="D54" s="67" t="s">
+      <c r="D54" s="69" t="s">
         <v>211</v>
       </c>
-      <c r="E54" s="69" t="s">
+      <c r="E54" s="71" t="s">
         <v>212</v>
       </c>
-      <c r="F54" s="67" t="s">
+      <c r="F54" s="69" t="s">
         <v>213</v>
       </c>
       <c r="G54" s="2" t="s">
@@ -5453,25 +5469,25 @@
       <c r="J54" s="2">
         <v>2030</v>
       </c>
-      <c r="K54" s="59">
-        <v>0</v>
-      </c>
-      <c r="L54" s="59">
+      <c r="K54" s="61">
+        <v>0</v>
+      </c>
+      <c r="L54" s="61">
         <v>1</v>
       </c>
-      <c r="M54" s="63">
+      <c r="M54" s="65">
         <v>0.5</v>
       </c>
-      <c r="N54" s="59">
+      <c r="N54" s="61">
         <v>0.5</v>
       </c>
-      <c r="O54" s="60">
+      <c r="O54" s="62">
         <v>0.7</v>
       </c>
-      <c r="P54" s="61" t="s">
+      <c r="P54" s="63" t="s">
         <v>418</v>
       </c>
-      <c r="Q54" s="61" t="s">
+      <c r="Q54" s="63" t="s">
         <v>418</v>
       </c>
       <c r="R54" s="28" t="s">
@@ -5482,12 +5498,12 @@
       </c>
     </row>
     <row r="55" spans="1:20" ht="72" customHeight="1">
-      <c r="A55" s="68"/>
-      <c r="B55" s="68"/>
-      <c r="C55" s="68"/>
-      <c r="D55" s="68"/>
-      <c r="E55" s="70"/>
-      <c r="F55" s="68"/>
+      <c r="A55" s="70"/>
+      <c r="B55" s="70"/>
+      <c r="C55" s="70"/>
+      <c r="D55" s="70"/>
+      <c r="E55" s="72"/>
+      <c r="F55" s="70"/>
       <c r="G55" s="2" t="s">
         <v>204</v>
       </c>
@@ -5501,13 +5517,13 @@
       <c r="J55" s="2">
         <v>2030</v>
       </c>
-      <c r="K55" s="59"/>
-      <c r="L55" s="59"/>
-      <c r="M55" s="64"/>
-      <c r="N55" s="59"/>
-      <c r="O55" s="60"/>
-      <c r="P55" s="61"/>
-      <c r="Q55" s="61"/>
+      <c r="K55" s="61"/>
+      <c r="L55" s="61"/>
+      <c r="M55" s="66"/>
+      <c r="N55" s="61"/>
+      <c r="O55" s="62"/>
+      <c r="P55" s="63"/>
+      <c r="Q55" s="63"/>
       <c r="R55" s="28" t="s">
         <v>368</v>
       </c>
@@ -5979,22 +5995,22 @@
       </c>
     </row>
     <row r="65" spans="1:19" ht="162.6" customHeight="1">
-      <c r="A65" s="2" t="s">
+      <c r="A65" s="28" t="s">
         <v>241</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B65" s="28" t="s">
         <v>253</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C65" s="28" t="s">
         <v>254</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="D65" s="28" t="s">
         <v>255</v>
       </c>
-      <c r="E65" s="27" t="s">
+      <c r="E65" s="56" t="s">
         <v>256</v>
       </c>
-      <c r="F65" s="2" t="s">
+      <c r="F65" s="28" t="s">
         <v>257</v>
       </c>
       <c r="G65" s="2" t="s">
@@ -6017,13 +6033,13 @@
         <v>1</v>
       </c>
       <c r="M65" s="3">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="N65" s="3">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="O65" s="16">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="P65" s="7" t="s">
         <v>422</v>
@@ -6039,22 +6055,22 @@
       </c>
     </row>
     <row r="66" spans="1:19" ht="72" customHeight="1">
-      <c r="A66" s="2" t="s">
+      <c r="A66" s="28" t="s">
         <v>241</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B66" s="28" t="s">
         <v>253</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C66" s="28" t="s">
         <v>258</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="D66" s="28" t="s">
         <v>259</v>
       </c>
-      <c r="E66" s="27" t="s">
+      <c r="E66" s="56" t="s">
         <v>260</v>
       </c>
-      <c r="F66" s="2" t="s">
+      <c r="F66" s="28" t="s">
         <v>261</v>
       </c>
       <c r="G66" s="7"/>
@@ -6070,10 +6086,10 @@
         <v>1</v>
       </c>
       <c r="M66" s="3">
-        <v>0.3</v>
+        <v>0.65</v>
       </c>
       <c r="N66" s="3">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="O66" s="16">
         <v>1</v>
@@ -6084,22 +6100,22 @@
       <c r="S66" s="2"/>
     </row>
     <row r="67" spans="1:19" ht="72" customHeight="1">
-      <c r="A67" s="11" t="s">
+      <c r="A67" s="57" t="s">
         <v>241</v>
       </c>
-      <c r="B67" s="11" t="s">
+      <c r="B67" s="57" t="s">
         <v>253</v>
       </c>
-      <c r="C67" s="11" t="s">
+      <c r="C67" s="57" t="s">
         <v>262</v>
       </c>
-      <c r="D67" s="11" t="s">
+      <c r="D67" s="57" t="s">
         <v>234</v>
       </c>
-      <c r="E67" s="30" t="s">
+      <c r="E67" s="58" t="s">
         <v>263</v>
       </c>
-      <c r="F67" s="11" t="s">
+      <c r="F67" s="57" t="s">
         <v>264</v>
       </c>
       <c r="G67" s="7"/>
@@ -6115,13 +6131,13 @@
         <v>1</v>
       </c>
       <c r="M67" s="3">
-        <v>0.3</v>
+        <v>0.65</v>
       </c>
       <c r="N67" s="3">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="O67" s="16">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
       <c r="P67" s="7" t="s">
         <v>265</v>
@@ -6137,22 +6153,22 @@
       </c>
     </row>
     <row r="68" spans="1:19" ht="72" customHeight="1">
-      <c r="A68" s="2" t="s">
+      <c r="A68" s="28" t="s">
         <v>241</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B68" s="28" t="s">
         <v>253</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C68" s="28" t="s">
         <v>267</v>
       </c>
-      <c r="D68" s="2" t="s">
+      <c r="D68" s="28" t="s">
         <v>268</v>
       </c>
-      <c r="E68" s="27" t="s">
+      <c r="E68" s="56" t="s">
         <v>269</v>
       </c>
-      <c r="F68" s="2" t="s">
+      <c r="F68" s="28" t="s">
         <v>270</v>
       </c>
       <c r="G68" s="7"/>
@@ -6168,13 +6184,13 @@
         <v>1</v>
       </c>
       <c r="M68" s="3">
-        <v>0.3</v>
+        <v>0.65</v>
       </c>
       <c r="N68" s="3">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="O68" s="16">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
       <c r="P68" s="7" t="s">
         <v>265</v>
@@ -6190,22 +6206,22 @@
       </c>
     </row>
     <row r="69" spans="1:19" ht="72" customHeight="1">
-      <c r="A69" s="11" t="s">
+      <c r="A69" s="83" t="s">
         <v>241</v>
       </c>
-      <c r="B69" s="11" t="s">
+      <c r="B69" s="83" t="s">
         <v>253</v>
       </c>
-      <c r="C69" s="11" t="s">
+      <c r="C69" s="83" t="s">
         <v>272</v>
       </c>
-      <c r="D69" s="11" t="s">
+      <c r="D69" s="83" t="s">
         <v>273</v>
       </c>
-      <c r="E69" s="30" t="s">
+      <c r="E69" s="84" t="s">
         <v>274</v>
       </c>
-      <c r="F69" s="11" t="s">
+      <c r="F69" s="83" t="s">
         <v>275</v>
       </c>
       <c r="G69" s="7"/>
@@ -6223,7 +6239,7 @@
       <c r="M69" s="3"/>
       <c r="N69" s="3"/>
       <c r="O69" s="16">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
       <c r="P69" s="15"/>
       <c r="Q69" s="7"/>
@@ -6235,22 +6251,22 @@
       </c>
     </row>
     <row r="70" spans="1:19" ht="72" customHeight="1">
-      <c r="A70" s="11" t="s">
+      <c r="A70" s="57" t="s">
         <v>241</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B70" s="28" t="s">
         <v>253</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C70" s="28" t="s">
         <v>276</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="D70" s="28" t="s">
         <v>277</v>
       </c>
-      <c r="E70" s="27" t="s">
+      <c r="E70" s="56" t="s">
         <v>278</v>
       </c>
-      <c r="F70" s="2" t="s">
+      <c r="F70" s="28" t="s">
         <v>279</v>
       </c>
       <c r="G70" s="7"/>
@@ -6266,10 +6282,10 @@
         <v>1</v>
       </c>
       <c r="M70" s="3">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="N70" s="3">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="O70" s="16">
         <v>1</v>
@@ -6286,22 +6302,22 @@
       </c>
     </row>
     <row r="71" spans="1:19" ht="171" customHeight="1">
-      <c r="A71" s="2" t="s">
+      <c r="A71" s="28" t="s">
         <v>241</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B71" s="28" t="s">
         <v>253</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C71" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D71" s="28" t="s">
         <v>282</v>
       </c>
-      <c r="E71" s="27" t="s">
+      <c r="E71" s="56" t="s">
         <v>283</v>
       </c>
-      <c r="F71" s="2" t="s">
+      <c r="F71" s="28" t="s">
         <v>284</v>
       </c>
       <c r="G71" s="2" t="s">
@@ -6323,9 +6339,11 @@
       <c r="L71" s="3" t="s">
         <v>633</v>
       </c>
-      <c r="M71" s="3"/>
+      <c r="M71" s="3">
+        <v>0.5</v>
+      </c>
       <c r="N71" s="3">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="O71" s="37">
         <v>0.95</v>
@@ -8760,9 +8778,9 @@
         <f>IF(VLOOKUP(D34,main!C:O,11,FALSE)=0,"",VLOOKUP(D34,main!C:O,11,FALSE))</f>
         <v/>
       </c>
-      <c r="F34" s="21">
+      <c r="F34" s="21" t="str">
         <f>IF(VLOOKUP(D34,main!C:O,12,FALSE)=0,"",VLOOKUP(D34,main!C:O,12,FALSE))</f>
-        <v>0.5</v>
+        <v/>
       </c>
       <c r="G34" s="21">
         <f>IF(VLOOKUP(D34,main!C:O,13,FALSE)=0,"",VLOOKUP(D34,main!C:O,13,FALSE))</f>
@@ -9330,15 +9348,15 @@
       </c>
       <c r="E56" s="21">
         <f>IF(VLOOKUP(D56,main!C:O,11,FALSE)=0,"",VLOOKUP(D56,main!C:O,11,FALSE))</f>
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="F56" s="21">
         <f>IF(VLOOKUP(D56,main!C:O,12,FALSE)=0,"",VLOOKUP(D56,main!C:O,12,FALSE))</f>
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="G56" s="21">
         <f>IF(VLOOKUP(D56,main!C:O,13,FALSE)=0,"",VLOOKUP(D56,main!C:O,13,FALSE))</f>
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -9356,11 +9374,11 @@
       </c>
       <c r="E57" s="21">
         <f>IF(VLOOKUP(D57,main!C:O,11,FALSE)=0,"",VLOOKUP(D57,main!C:O,11,FALSE))</f>
-        <v>0.3</v>
+        <v>0.65</v>
       </c>
       <c r="F57" s="21">
         <f>IF(VLOOKUP(D57,main!C:O,12,FALSE)=0,"",VLOOKUP(D57,main!C:O,12,FALSE))</f>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="G57" s="21">
         <f>IF(VLOOKUP(D57,main!C:O,13,FALSE)=0,"",VLOOKUP(D57,main!C:O,13,FALSE))</f>
@@ -9382,15 +9400,15 @@
       </c>
       <c r="E58" s="21">
         <f>IF(VLOOKUP(D58,main!C:O,11,FALSE)=0,"",VLOOKUP(D58,main!C:O,11,FALSE))</f>
-        <v>0.3</v>
+        <v>0.65</v>
       </c>
       <c r="F58" s="21">
         <f>IF(VLOOKUP(D58,main!C:O,12,FALSE)=0,"",VLOOKUP(D58,main!C:O,12,FALSE))</f>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="G58" s="21">
         <f>IF(VLOOKUP(D58,main!C:O,13,FALSE)=0,"",VLOOKUP(D58,main!C:O,13,FALSE))</f>
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -9408,15 +9426,15 @@
       </c>
       <c r="E59" s="21">
         <f>IF(VLOOKUP(D59,main!C:O,11,FALSE)=0,"",VLOOKUP(D59,main!C:O,11,FALSE))</f>
-        <v>0.3</v>
+        <v>0.65</v>
       </c>
       <c r="F59" s="21">
         <f>IF(VLOOKUP(D59,main!C:O,12,FALSE)=0,"",VLOOKUP(D59,main!C:O,12,FALSE))</f>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="G59" s="21">
         <f>IF(VLOOKUP(D59,main!C:O,13,FALSE)=0,"",VLOOKUP(D59,main!C:O,13,FALSE))</f>
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -9442,7 +9460,7 @@
       </c>
       <c r="G60" s="21">
         <f>IF(VLOOKUP(D60,main!C:O,13,FALSE)=0,"",VLOOKUP(D60,main!C:O,13,FALSE))</f>
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -9460,11 +9478,11 @@
       </c>
       <c r="E61" s="21">
         <f>IF(VLOOKUP(D61,main!C:O,11,FALSE)=0,"",VLOOKUP(D61,main!C:O,11,FALSE))</f>
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="F61" s="21">
         <f>IF(VLOOKUP(D61,main!C:O,12,FALSE)=0,"",VLOOKUP(D61,main!C:O,12,FALSE))</f>
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="G61" s="21">
         <f>IF(VLOOKUP(D61,main!C:O,13,FALSE)=0,"",VLOOKUP(D61,main!C:O,13,FALSE))</f>
@@ -9484,13 +9502,13 @@
       <c r="D62" s="10" t="s">
         <v>281</v>
       </c>
-      <c r="E62" s="21" t="str">
+      <c r="E62" s="21">
         <f>IF(VLOOKUP(D62,main!C:O,11,FALSE)=0,"",VLOOKUP(D62,main!C:O,11,FALSE))</f>
-        <v/>
+        <v>0.5</v>
       </c>
       <c r="F62" s="21">
         <f>IF(VLOOKUP(D62,main!C:O,12,FALSE)=0,"",VLOOKUP(D62,main!C:O,12,FALSE))</f>
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="G62" s="21">
         <f>IF(VLOOKUP(D62,main!C:O,13,FALSE)=0,"",VLOOKUP(D62,main!C:O,13,FALSE))</f>

</xml_diff>